<commit_message>
Auto update photos 2025-11-26 09:49:54
</commit_message>
<xml_diff>
--- a/photo_links.xlsx
+++ b/photo_links.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2504_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2504_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2505_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2505_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2506_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2506_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2507_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2507_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -549,7 +549,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2508_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2508_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -571,7 +571,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2509_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2509_image_005.jpg</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\005\2510_image_005.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212/005\2510_image_005.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2025-11-26 10:22:09
</commit_message>
<xml_diff>
--- a/photo_links.xlsx
+++ b/photo_links.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,16 @@
           <t>Local file</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Width</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -461,8 +471,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2504_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2504_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>900</v>
+      </c>
+      <c r="F2" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="3">
@@ -483,8 +499,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2505_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2505_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>900</v>
+      </c>
+      <c r="F3" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="4">
@@ -505,8 +527,14 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2506_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2506_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>900</v>
+      </c>
+      <c r="F4" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="5">
@@ -527,8 +555,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2507_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2507_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>900</v>
+      </c>
+      <c r="F5" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="6">
@@ -549,8 +583,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2508_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2508_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>900</v>
+      </c>
+      <c r="F6" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="7">
@@ -571,8 +611,14 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2509_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2509_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>900</v>
+      </c>
+      <c r="F7" t="n">
+        <v>900</v>
       </c>
     </row>
     <row r="8">
@@ -593,8 +639,14 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212/005\2510_image_005.jpg</t>
-        </is>
+          <t>C:/Users/Asus/Desktop/21212\005\2510_image_005.jpg</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>900</v>
+      </c>
+      <c r="F8" t="n">
+        <v>900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-11-26 19:20:57
</commit_message>
<xml_diff>
--- a/photo_links.xlsx
+++ b/photo_links.xlsx
@@ -18124,7 +18124,7 @@
     <row r="633">
       <c r="A633" t="inlineStr">
         <is>
-          <t>8062-green-pixel_1</t>
+          <t>8062-green-pixel</t>
         </is>
       </c>
       <c r="B633" t="inlineStr">
@@ -18134,12 +18134,12 @@
       </c>
       <c r="C633" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel_1/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/1.jpg</t>
         </is>
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\1_image_8062-green-pixel_1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\1_image_8062-green-pixel.jpg</t>
         </is>
       </c>
       <c r="E633" t="n">
@@ -18180,29 +18180,29 @@
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>8062-green-pixel_1</t>
+          <t>8062-green-pixel</t>
         </is>
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>2.jpg</t>
+          <t>3.jpg</t>
         </is>
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel_1/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/3.jpg</t>
         </is>
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\2_image_8062-green-pixel_1.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\3_image_8062-green-pixel.jpg</t>
         </is>
       </c>
       <c r="E635" t="n">
-        <v>900</v>
+        <v>829</v>
       </c>
       <c r="F635" t="n">
-        <v>900</v>
+        <v>757</v>
       </c>
     </row>
     <row r="636">
@@ -18213,24 +18213,24 @@
       </c>
       <c r="B636" t="inlineStr">
         <is>
-          <t>3.jpg</t>
+          <t>4.jpg</t>
         </is>
       </c>
       <c r="C636" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/4.jpg</t>
         </is>
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\3_image_8062-green-pixel.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\4_image_8062-green-pixel.jpg</t>
         </is>
       </c>
       <c r="E636" t="n">
-        <v>829</v>
+        <v>561</v>
       </c>
       <c r="F636" t="n">
-        <v>757</v>
+        <v>839</v>
       </c>
     </row>
     <row r="637">
@@ -18241,24 +18241,24 @@
       </c>
       <c r="B637" t="inlineStr">
         <is>
-          <t>4.jpg</t>
+          <t>5.jpg</t>
         </is>
       </c>
       <c r="C637" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/5.jpg</t>
         </is>
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\4_image_8062-green-pixel.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\5_image_8062-green-pixel.jpg</t>
         </is>
       </c>
       <c r="E637" t="n">
-        <v>561</v>
+        <v>900</v>
       </c>
       <c r="F637" t="n">
-        <v>839</v>
+        <v>900</v>
       </c>
     </row>
     <row r="638">
@@ -18269,17 +18269,17 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>5.jpg</t>
+          <t>6.jpg</t>
         </is>
       </c>
       <c r="C638" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8062-green-pixel/6.jpg</t>
         </is>
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\5_image_8062-green-pixel.jpg</t>
+          <t>C:/Users/Asus/Desktop/21212\8062-green-pixel\6_image_8062-green-pixel.jpg</t>
         </is>
       </c>
       <c r="E638" t="n">

</xml_diff>